<commit_message>
19_12_12 @ 10:11 ReadMeExcel file updated
</commit_message>
<xml_diff>
--- a/excel files /Project excel files /1. Excel_ReadMe_File.xlsx
+++ b/excel files /Project excel files /1. Excel_ReadMe_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasondalrymple/Desktop/CASA2019_Assignment/excel files /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasondalrymple/Desktop/CASA_Assignment_2019/excel files /Project excel files /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6824E49-02AB-2547-9FA3-53EE26905A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BD6E399-5CAC-C44C-92C0-1C7BFAD2BCB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="460" windowWidth="27640" windowHeight="16020" xr2:uid="{98394905-928A-704B-89B3-CE94A036B0DC}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16020" xr2:uid="{98394905-928A-704B-89B3-CE94A036B0DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>@Jason Dalrymple</t>
   </si>
@@ -39,18 +39,9 @@
     <t>23 November 2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Each tap in this spreadsheet contains a set of data that has been used as part of the Analysis of the possible options for the Bakerloo Lines. </t>
-  </si>
-  <si>
-    <t>The report called " An Examination as to whether the right route has been selected for the proposed Bakerloo Line Extension" makes reference</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>6 Graphs</t>
-  </si>
-  <si>
     <t>2.1 Route1_Station_Coordinates</t>
   </si>
   <si>
@@ -126,13 +117,16 @@
     <t>Contains Route 2 data on Transport access scores and employment IMD scores - combined and indexed to R1</t>
   </si>
   <si>
-    <t xml:space="preserve">to a number of different excel files (which may have been originally exported from the shapefile as CVS files), or from which data has been extracted, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">and manipulated to create separate datasets or spreadsheets. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Flowchart boxes have html links to relevant files </t>
+    <t xml:space="preserve">This file describes the analyitical process undertaken to examine the relationship between Wards &amp; LSOA's along the BLE Routes 1 &amp; 2. </t>
+  </si>
+  <si>
+    <t>There are a number of files in the github repository, each of which is numbered sequentially, and the purpose of each is described in the flow chart below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each blue bo contains a html link to the relevant files. </t>
+  </si>
+  <si>
+    <t>4. Graphs</t>
   </si>
 </sst>
 </file>
@@ -1281,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F856E6-34DD-E447-9A7B-29BCA2838462}">
   <dimension ref="B2:P40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1309,27 +1303,27 @@
     </row>
     <row r="5" spans="2:16">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:16">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:16">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="16" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -1367,16 +1361,16 @@
     <row r="14" spans="2:16" ht="17">
       <c r="B14" s="5"/>
       <c r="C14" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P14" s="6"/>
     </row>
@@ -1393,10 +1387,10 @@
     <row r="17" spans="2:16" ht="27" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P17" s="6"/>
     </row>
@@ -1408,10 +1402,10 @@
     <row r="19" spans="2:16" ht="27" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P19" s="6"/>
     </row>
@@ -1423,10 +1417,10 @@
     <row r="21" spans="2:16" ht="27" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P21" s="6"/>
     </row>
@@ -1434,14 +1428,14 @@
       <c r="B22" s="5"/>
       <c r="C22" s="13"/>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P22" s="6"/>
     </row>
     <row r="23" spans="2:16" ht="27" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P23" s="6"/>
     </row>
@@ -1453,10 +1447,10 @@
     <row r="25" spans="2:16" ht="27" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P25" s="6"/>
     </row>
@@ -1468,10 +1462,10 @@
     <row r="27" spans="2:16" ht="27" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="12" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P27" s="6"/>
     </row>
@@ -1483,10 +1477,10 @@
     <row r="29" spans="2:16" ht="27" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P29" s="6"/>
     </row>
@@ -1498,10 +1492,10 @@
     <row r="31" spans="2:16" ht="27" customHeight="1">
       <c r="B31" s="5"/>
       <c r="C31" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P31" s="6"/>
     </row>
@@ -1513,10 +1507,10 @@
     <row r="33" spans="2:16" ht="27" customHeight="1">
       <c r="B33" s="5"/>
       <c r="C33" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="P33" s="6"/>
     </row>
@@ -1524,17 +1518,17 @@
       <c r="B34" s="5"/>
       <c r="C34" s="13"/>
       <c r="G34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P34" s="6"/>
     </row>
     <row r="35" spans="2:16" ht="27" customHeight="1">
       <c r="B35" s="5"/>
       <c r="C35" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P35" s="6"/>
     </row>
@@ -1546,10 +1540,10 @@
     <row r="37" spans="2:16" ht="27" customHeight="1">
       <c r="B37" s="5"/>
       <c r="C37" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="P37" s="6"/>
     </row>
@@ -1561,10 +1555,10 @@
     <row r="39" spans="2:16" ht="27" customHeight="1">
       <c r="B39" s="5"/>
       <c r="C39" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="P39" s="6"/>
     </row>
@@ -1575,7 +1569,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
@@ -1592,18 +1586,18 @@
     <mergeCell ref="B10:P10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C25" r:id="rId1" display="5. R2 Buffer Data" xr:uid="{BE90B63A-271B-8045-AC09-698FB9A4FEF9}"/>
-    <hyperlink ref="C29" r:id="rId2" display="7. Transport Access Scores " xr:uid="{A5E8A437-8D45-7B46-9FCE-2FB581E8EC54}"/>
+    <hyperlink ref="C25" r:id="rId1" xr:uid="{BE90B63A-271B-8045-AC09-698FB9A4FEF9}"/>
+    <hyperlink ref="C29" r:id="rId2" xr:uid="{A5E8A437-8D45-7B46-9FCE-2FB581E8EC54}"/>
     <hyperlink ref="C27" r:id="rId3" xr:uid="{E7C500DB-E93B-9B4E-9CBA-770281C8393C}"/>
-    <hyperlink ref="C23" r:id="rId4" display="3.2 Route1_Buffer_Data" xr:uid="{9E73E4B5-93E7-DA4C-9E10-064D820756C7}"/>
-    <hyperlink ref="C21" r:id="rId5" display="3. Employment IMD Scores " xr:uid="{CEB89AB3-E5B9-D44E-A987-CB4B80D0A2C6}"/>
-    <hyperlink ref="C19" r:id="rId6" display="2. R2 Stations" xr:uid="{BAEE23F2-231B-4747-9BD6-51D6C5C66962}"/>
-    <hyperlink ref="C17" r:id="rId7" display="1. R1 Station" xr:uid="{8C088B25-5293-724D-A8DE-E6D9E288388A}"/>
-    <hyperlink ref="C31" r:id="rId8" display="8 TAS R1 &amp; R2" xr:uid="{20583200-357C-B542-88A5-964FA39D64EF}"/>
-    <hyperlink ref="C33" r:id="rId9" display="9. Emp @ Ward leve" xr:uid="{A8655801-08C6-1448-A329-0942C9C00308}"/>
-    <hyperlink ref="C35" r:id="rId10" display="10 R2 Emp &amp; TAS indexed" xr:uid="{88E93C0E-809D-7842-9A2D-B6A1BD856E54}"/>
-    <hyperlink ref="C39" r:id="rId11" display="9.2 Data for new R2 stations.xlsx" xr:uid="{A2E6F6D0-A190-8F43-BE60-2447FBA8694E}"/>
-    <hyperlink ref="C37" r:id="rId12" display="9.1 Data for new R1 stations.xlsx" xr:uid="{4D943177-BE7A-0545-8381-0945008DD781}"/>
+    <hyperlink ref="C23" r:id="rId4" xr:uid="{9E73E4B5-93E7-DA4C-9E10-064D820756C7}"/>
+    <hyperlink ref="C21" r:id="rId5" xr:uid="{CEB89AB3-E5B9-D44E-A987-CB4B80D0A2C6}"/>
+    <hyperlink ref="C19" r:id="rId6" xr:uid="{BAEE23F2-231B-4747-9BD6-51D6C5C66962}"/>
+    <hyperlink ref="C17" r:id="rId7" xr:uid="{8C088B25-5293-724D-A8DE-E6D9E288388A}"/>
+    <hyperlink ref="C31" r:id="rId8" xr:uid="{20583200-357C-B542-88A5-964FA39D64EF}"/>
+    <hyperlink ref="C33" r:id="rId9" xr:uid="{A8655801-08C6-1448-A329-0942C9C00308}"/>
+    <hyperlink ref="C35" r:id="rId10" xr:uid="{88E93C0E-809D-7842-9A2D-B6A1BD856E54}"/>
+    <hyperlink ref="C39" r:id="rId11" xr:uid="{A2E6F6D0-A190-8F43-BE60-2447FBA8694E}"/>
+    <hyperlink ref="C37" r:id="rId12" xr:uid="{4D943177-BE7A-0545-8381-0945008DD781}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId13"/>

</xml_diff>